<commit_message>
correct data + add slides
</commit_message>
<xml_diff>
--- a/files/QT2/exo_lec4.xlsx
+++ b/files/QT2/exo_lec4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisdecharson/Desktop/Sciences-Po/Enseignement/QT level 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisdecharson/Documents/github/louisdecharson.github.io/files/QT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Quarter</t>
   </si>
@@ -397,22 +397,18 @@
       <t xml:space="preserve"> inflation.</t>
     </r>
   </si>
+  <si>
+    <t>HICP (q-o-q, annualized)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,20 +476,20 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -892,18 +888,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>7</v>
@@ -914,8 +911,11 @@
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -928,11 +928,12 @@
       <c r="D2" s="8">
         <v>18.57</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="8"/>
+      <c r="G2" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -945,12 +946,15 @@
       <c r="D3" s="8">
         <v>19.5</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="8">
+        <v>1.9705200502173099</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -963,13 +967,16 @@
       <c r="D4" s="8">
         <v>20.9</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="8">
+        <v>0.90721327458206502</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -982,13 +989,16 @@
       <c r="D5" s="8">
         <v>23.57</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="8">
+        <v>1.77964618357598</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1001,13 +1011,16 @@
       <c r="D6" s="8">
         <v>21.17</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="8">
+        <v>2.4867266986846999</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1020,13 +1033,16 @@
       <c r="D7" s="8">
         <v>18.05</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="8">
+        <v>0.20775165734641299</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1039,13 +1055,16 @@
       <c r="D8" s="8">
         <v>18.510000000000002</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="8">
+        <v>1.8307321417547699</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1058,13 +1077,16 @@
       <c r="D9" s="8">
         <v>18.739999999999998</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="8">
+        <v>1.5921591758092799</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1077,10 +1099,13 @@
       <c r="D10" s="8">
         <v>14.12</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="8">
+        <v>0.80027377690527801</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1093,10 +1118,13 @@
       <c r="D11" s="8">
         <v>13.37</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="8">
+        <v>1.09816232225541</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -1109,10 +1137,13 @@
       <c r="D12" s="8">
         <v>12.44</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="8">
+        <v>1.0157245122715901</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1125,10 +1156,13 @@
       <c r="D13" s="8">
         <v>11.19</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="8">
+        <v>0.36409274767618799</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -1141,10 +1175,13 @@
       <c r="D14" s="8">
         <v>11.3</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="8">
+        <v>0.77443129479256301</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
@@ -1157,10 +1194,13 @@
       <c r="D15" s="8">
         <v>15.46</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="8">
+        <v>1.5944375036990299</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -1173,10 +1213,13 @@
       <c r="D16" s="8">
         <v>20.61</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16" s="8">
+        <v>1.7654846763208201</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -1189,10 +1232,13 @@
       <c r="D17" s="8">
         <v>24.02</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E17" s="8">
+        <v>1.8346897779587199</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1205,10 +1251,13 @@
       <c r="D18" s="8">
         <v>26.93</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E18" s="8">
+        <v>2.4371226218662101</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
@@ -1221,10 +1270,13 @@
       <c r="D19" s="8">
         <v>26.77</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E19" s="8">
+        <v>1.2514961215565299</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -1237,10 +1289,13 @@
       <c r="D20" s="8">
         <v>30.67</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="8">
+        <v>3.2251154324322999</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>29</v>
       </c>
@@ -1253,10 +1308,13 @@
       <c r="D21" s="8">
         <v>29.72</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E21" s="8">
+        <v>2.7206694248694299</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -1269,10 +1327,13 @@
       <c r="D22" s="8">
         <v>25.87</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E22" s="8">
+        <v>1.0236831860453</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
@@ -1285,10 +1346,13 @@
       <c r="D23" s="8">
         <v>27.27</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E23" s="8">
+        <v>4.2924534599558299</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
@@ -1301,10 +1365,13 @@
       <c r="D24" s="8">
         <v>25.3</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="8">
+        <v>1.2880176851629801</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
@@ -1317,10 +1384,13 @@
       <c r="D25" s="8">
         <v>19.350000000000001</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="8">
+        <v>1.6416823705756001</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>34</v>
       </c>
@@ -1333,10 +1403,13 @@
       <c r="D26" s="8">
         <v>21.13</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E26" s="8">
+        <v>2.8711251136193798</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>35</v>
       </c>
@@ -1349,10 +1422,13 @@
       <c r="D27" s="8">
         <v>25.05</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E27" s="8">
+        <v>2.3434751942188501</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>36</v>
       </c>
@@ -1365,10 +1441,13 @@
       <c r="D28" s="8">
         <v>26.93</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E28" s="8">
+        <v>1.5091231276439101</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
@@ -1381,10 +1460,13 @@
       <c r="D29" s="8">
         <v>26.74</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E29" s="8">
+        <v>2.2247063599927399</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>38</v>
       </c>
@@ -1397,10 +1479,13 @@
       <c r="D30" s="8">
         <v>31.52</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="8">
+        <v>3.14399879663755</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>39</v>
       </c>
@@ -1413,10 +1498,13 @@
       <c r="D31" s="8">
         <v>26.17</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E31" s="8">
+        <v>0.72450602912523898</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
@@ -1429,10 +1517,13 @@
       <c r="D32" s="8">
         <v>28.45</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E32" s="8">
+        <v>1.9456273910246999</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>41</v>
       </c>
@@ -1445,10 +1536,13 @@
       <c r="D33" s="8">
         <v>29.39</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E33" s="8">
+        <v>2.2218095229870198</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
@@ -1461,10 +1555,13 @@
       <c r="D34" s="8">
         <v>31.92</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E34" s="8">
+        <v>2.1397718998398698</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>43</v>
       </c>
@@ -1477,10 +1574,13 @@
       <c r="D35" s="8">
         <v>35.450000000000003</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E35" s="8">
+        <v>2.6476220355200799</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>44</v>
       </c>
@@ -1493,10 +1593,13 @@
       <c r="D36" s="8">
         <v>41.39</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E36" s="8">
+        <v>1.9235322792424401</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>45</v>
       </c>
@@ -1509,10 +1612,13 @@
       <c r="D37" s="8">
         <v>44.16</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E37" s="8">
+        <v>2.29815121991833</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>46</v>
       </c>
@@ -1525,10 +1631,13 @@
       <c r="D38" s="8">
         <v>47.7</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E38" s="8">
+        <v>1.4709070931396699</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>47</v>
       </c>
@@ -1541,10 +1650,13 @@
       <c r="D39" s="8">
         <v>51.63</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E39" s="8">
+        <v>2.2341119953753399</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>48</v>
       </c>
@@ -1557,10 +1669,13 @@
       <c r="D40" s="8">
         <v>61.47</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E40" s="8">
+        <v>3.0935597608970702</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>49</v>
       </c>
@@ -1573,10 +1688,13 @@
       <c r="D41" s="8">
         <v>56.88</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E41" s="8">
+        <v>2.3558077921185201</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>50</v>
       </c>
@@ -1589,10 +1707,13 @@
       <c r="D42" s="8">
         <v>61.75</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E42" s="8">
+        <v>1.6961797558056599</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>51</v>
       </c>
@@ -1605,10 +1726,13 @@
       <c r="D43" s="8">
         <v>69.53</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E43" s="8">
+        <v>2.4549368138366301</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>52</v>
       </c>
@@ -1621,10 +1745,13 @@
       <c r="D44" s="8">
         <v>69.62</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E44" s="8">
+        <v>2.0739410487879</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>53</v>
       </c>
@@ -1637,10 +1764,13 @@
       <c r="D45" s="8">
         <v>59.68</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E45" s="8">
+        <v>0.79483110199659801</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>54</v>
       </c>
@@ -1653,10 +1783,13 @@
       <c r="D46" s="8">
         <v>57.76</v>
       </c>
-      <c r="E46" s="7"/>
-      <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E46" s="8">
+        <v>2.25420919383824</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>55</v>
       </c>
@@ -1669,10 +1802,13 @@
       <c r="D47" s="8">
         <v>68.58</v>
       </c>
-      <c r="E47" s="7"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E47" s="8">
+        <v>2.2627551532701502</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>56</v>
       </c>
@@ -1685,10 +1821,13 @@
       <c r="D48" s="8">
         <v>74.95</v>
       </c>
-      <c r="E48" s="7"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E48" s="8">
+        <v>2.1741654203853602</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>57</v>
       </c>
@@ -1701,10 +1840,13 @@
       <c r="D49" s="8">
         <v>88.56</v>
       </c>
-      <c r="E49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E49" s="8">
+        <v>4.6739796939242497</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>58</v>
       </c>
@@ -1717,10 +1859,13 @@
       <c r="D50" s="8">
         <v>96.94</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E50" s="8">
+        <v>4.1225441191343899</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>59</v>
       </c>
@@ -1733,10 +1878,13 @@
       <c r="D51" s="8">
         <v>121.4</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E51" s="8">
+        <v>3.2109735773891801</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>60</v>
       </c>
@@ -1749,10 +1897,13 @@
       <c r="D52" s="8">
         <v>114.4</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E52" s="8">
+        <v>3.1883623586044898</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>61</v>
       </c>
@@ -1765,10 +1916,13 @@
       <c r="D53" s="8">
         <v>54.66</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E53" s="8">
+        <v>-1.5096282855054</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>62</v>
       </c>
@@ -1781,10 +1935,13 @@
       <c r="D54" s="8">
         <v>44.43</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="G54" s="7"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E54" s="8">
+        <v>-1.1076678385965599</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>63</v>
       </c>
@@ -1797,10 +1954,13 @@
       <c r="D55" s="8">
         <v>58.7</v>
       </c>
-      <c r="E55" s="7"/>
-      <c r="G55" s="7"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E55" s="8">
+        <v>5.3433266386156301E-2</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>64</v>
       </c>
@@ -1813,10 +1973,13 @@
       <c r="D56" s="8">
         <v>68.2</v>
       </c>
-      <c r="E56" s="7"/>
-      <c r="G56" s="7"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E56" s="8">
+        <v>1.15565114357093</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>65</v>
       </c>
@@ -1829,10 +1992,13 @@
       <c r="D57" s="8">
         <v>74.63</v>
       </c>
-      <c r="E57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E57" s="8">
+        <v>1.52879415874026</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>66</v>
       </c>
@@ -1845,10 +2011,13 @@
       <c r="D58" s="8">
         <v>76.25</v>
       </c>
-      <c r="E58" s="7"/>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E58" s="8">
+        <v>1.72686409208113</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>67</v>
       </c>
@@ -1861,10 +2030,13 @@
       <c r="D59" s="8">
         <v>78.510000000000005</v>
       </c>
-      <c r="E59" s="7"/>
-      <c r="G59" s="7"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E59" s="8">
+        <v>1.99324566136371</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>68</v>
       </c>
@@ -1877,10 +2049,13 @@
       <c r="D60" s="8">
         <v>76.819999999999993</v>
       </c>
-      <c r="E60" s="7"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E60" s="8">
+        <v>1.6551260802827801</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>69</v>
       </c>
@@ -1893,10 +2068,13 @@
       <c r="D61" s="8">
         <v>86.47</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E61" s="8">
+        <v>2.5193804437420799</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>70</v>
       </c>
@@ -1909,10 +2087,13 @@
       <c r="D62" s="8">
         <v>104.96</v>
       </c>
-      <c r="E62" s="7"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E62" s="8">
+        <v>3.5811172692760298</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>71</v>
       </c>
@@ -1925,10 +2106,13 @@
       <c r="D63" s="8">
         <v>117.36</v>
       </c>
-      <c r="E63" s="7"/>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E63" s="8">
+        <v>3.1733634924934599</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>72</v>
       </c>
@@ -1941,10 +2125,13 @@
       <c r="D64" s="8">
         <v>113.34</v>
       </c>
-      <c r="E64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E64" s="8">
+        <v>1.3539905538954899</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>73</v>
       </c>
@@ -1957,10 +2144,13 @@
       <c r="D65" s="8">
         <v>109.4</v>
       </c>
-      <c r="E65" s="7"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E65" s="8">
+        <v>3.3685978712334799</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>74</v>
       </c>
@@ -1973,10 +2163,13 @@
       <c r="D66" s="8">
         <v>118.49</v>
       </c>
-      <c r="E66" s="7"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E66" s="8">
+        <v>2.7555753489419099</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>75</v>
       </c>
@@ -1989,10 +2182,13 @@
       <c r="D67" s="8">
         <v>108.42</v>
       </c>
-      <c r="E67" s="7"/>
-      <c r="G67" s="7"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E67" s="8">
+        <v>2.3197710407311698</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>76</v>
       </c>
@@ -2005,10 +2201,13 @@
       <c r="D68" s="8">
         <v>109.61</v>
       </c>
-      <c r="E68" s="7"/>
-      <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E68" s="8">
+        <v>1.5803625347791801</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>77</v>
       </c>
@@ -2021,10 +2220,13 @@
       <c r="D69" s="8">
         <v>110.09</v>
       </c>
-      <c r="E69" s="7"/>
-      <c r="G69" s="7"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E69" s="8">
+        <v>2.31992012620162</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>78</v>
       </c>
@@ -2037,10 +2239,13 @@
       <c r="D70" s="8">
         <v>112.49</v>
       </c>
-      <c r="E70" s="7"/>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E70" s="8">
+        <v>1.2768153812085099</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>79</v>
       </c>
@@ -2053,9 +2258,12 @@
       <c r="D71" s="8">
         <v>102.58</v>
       </c>
-      <c r="G71" s="7"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E71" s="8">
+        <v>0.45681718232131902</v>
+      </c>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2068,8 +2276,11 @@
       <c r="D72" s="8">
         <v>110.27</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E72" s="8">
+        <v>1.19420641456828</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2082,8 +2293,11 @@
       <c r="D73" s="8">
         <v>109.21</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E73" s="8">
+        <v>0.190954004750786</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2096,8 +2310,11 @@
       <c r="D74" s="8">
         <v>108.17</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E74" s="8">
+        <v>0.92506237035226802</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2110,8 +2327,11 @@
       <c r="D75" s="8">
         <v>109.7</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E75" s="8">
+        <v>2.7885172035806401E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2124,8 +2344,11 @@
       <c r="D76" s="8">
         <v>101.82</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E76" s="8">
+        <v>0.18140129637039701</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2138,8 +2361,11 @@
       <c r="D77" s="8">
         <v>76.400000000000006</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E77" s="8">
+        <v>-0.537528310783143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2152,8 +2378,11 @@
       <c r="D78" s="8">
         <v>53.92</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E78" s="8">
+        <v>-0.75114114555269695</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2166,8 +2395,11 @@
       <c r="D79" s="8">
         <v>61.69</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E79" s="8">
+        <v>1.87562192360646</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2180,8 +2412,11 @@
       <c r="D80" s="8">
         <v>50.23</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="8">
+        <v>-0.30685714859319302</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2194,8 +2429,11 @@
       <c r="D81" s="8">
         <v>43.57</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="8">
+        <v>-0.18158904475447801</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2208,8 +2446,11 @@
       <c r="D82" s="8">
         <v>33.700000000000003</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="8">
+        <v>-1.14271846256888</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2222,8 +2463,11 @@
       <c r="D83" s="8">
         <v>45.52</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="8">
+        <v>1.2914318170271999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2236,8 +2480,11 @@
       <c r="D84" s="8">
         <v>45.79</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="8">
+        <v>1.0783966744042099</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2249,6 +2496,9 @@
       </c>
       <c r="D85" s="8">
         <v>49.18</v>
+      </c>
+      <c r="E85" s="8">
+        <v>1.7186390235179401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>